<commit_message>
Update questions, add admin password protection, and add entry instructions
</commit_message>
<xml_diff>
--- a/Super Bowl LX Picks.xlsx
+++ b/Super Bowl LX Picks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Timestamp</t>
   </si>
@@ -23,7 +23,7 @@
   </si>
   <si>
     <r>
-      <t>Seattle Seahawks (-4.5) @ New England Patriots -</t>
+      <t>Seattle Seahawks (-4.5) vs New England Patriots -</t>
     </r>
     <r>
       <rPr>
@@ -62,7 +62,7 @@
     <t>Jersey Number of First TD Scored: Over/Under 10.5</t>
   </si>
   <si>
-    <t>Drake Maye (NE) Passing Yards: Over/Under 223.5 Passing Yards</t>
+    <t>Drake Maye (NE) Passing Yards: Over/Under 223.5</t>
   </si>
   <si>
     <t>Sam Darnold (Sea) Passing Touchdowns: Over/Under 1.5</t>
@@ -83,7 +83,7 @@
     <t>Who will have more receiving yards? Hunter Henry (NE) or Cooper Kupp (Sea)</t>
   </si>
   <si>
-    <t>More Total Tackles: Christian Elliss (NE) or Nick Emmanwori</t>
+    <t>More Total Tackles: Christian Elliss (NE) or Nick Emmanwori (Sea)</t>
   </si>
   <si>
     <t>Will Both Teams Make 34 Yard or Longer Field Goal?</t>
@@ -125,13 +125,13 @@
     <t>From kick-off to end of regulation, will price of Bitcoin go up or down?</t>
   </si>
   <si>
-    <t>Will Kendrick Lamar be wearing a hoodie in opening appearance?</t>
-  </si>
-  <si>
-    <t>Kendrick Lamar First Song</t>
-  </si>
-  <si>
-    <t>Will Kendrick Lamar say the word "Pedophile" during the Halftime Show? (Kendrick must say it, does not count for back-up vocals)</t>
+    <t>Will Bad Bunny Make a Political Statement during the Halftime Show? (my interpretation)</t>
+  </si>
+  <si>
+    <t>Bad Bunny First Song</t>
+  </si>
+  <si>
+    <t>Will Bad Bunny wear a dress?</t>
   </si>
   <si>
     <t>Total Songs during Halftime Show: Over/Under 10.5</t>
@@ -143,47 +143,32 @@
     <t>Color of Gatorade bath for Head Coach of winning team:</t>
   </si>
   <si>
-    <t>Who will MVP mention first?</t>
+    <t>Who will MVP mention first? (after accepting award)</t>
   </si>
   <si>
     <t>TIE BREAKER -  Total Points Scored (Price is Right Rules - As close as you can without going over)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Would you like to opt-in for $20 SUPER BOWL POOL - Half of winnings go to charity of winner's choice and other half in their pocker.  Send a $20 Venmo to </t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>@john-deely-67</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Did you Venmo $20 to </t>
-    </r>
-    <r>
-      <rPr>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>@john-deely-67</t>
-    </r>
+    <t>Would you like to opt-in for $20 SUPER BOWL POOL - Half of winnings go to charity of winner's choice and other half in their pocket.  Send a $20 Venmo to @tim-roberts-16</t>
+  </si>
+  <si>
+    <t>Did you Venmo $20 to  @tim-roberts-16</t>
   </si>
   <si>
     <t>For auditing purposes, what is your Venmo handle? (Please include @ in the handle or just Venmo me)</t>
   </si>
   <si>
     <t>If you win, what is your charity of choice? (Please don't say "idk" like Aaron Black)</t>
+  </si>
+  <si>
+    <t>Will Cardi B perform at the Halftime Show?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -194,10 +179,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <color rgb="FF0000FF"/>
-      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,7 +202,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -303,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AT1" displayName="Form_Responses" name="Form_Responses" id="1">
-  <tableColumns count="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:AU1" displayName="Form_Responses" name="Form_Responses" id="1">
+  <tableColumns count="47">
     <tableColumn name="Column1" id="1"/>
     <tableColumn name="Column2" id="2"/>
     <tableColumn name="Column3" id="3"/>
@@ -351,6 +332,7 @@
     <tableColumn name="Column44" id="44"/>
     <tableColumn name="Column45" id="45"/>
     <tableColumn name="Column46" id="46"/>
+    <tableColumn name="Column47" id="47"/>
   </tableColumns>
   <tableStyleInfo name="Form Responses 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
   <extLst>
@@ -586,7 +568,7 @@
     <col customWidth="1" min="42" max="43" width="37.63"/>
     <col customWidth="1" min="44" max="44" width="32.75"/>
     <col customWidth="1" min="45" max="46" width="37.63"/>
-    <col customWidth="1" min="47" max="52" width="18.88"/>
+    <col customWidth="1" min="47" max="53" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="22.5" customHeight="1">
@@ -716,10 +698,10 @@
       <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AS1" s="1" t="s">
@@ -728,15 +710,14 @@
       <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="AQ1"/>
-    <hyperlink r:id="rId2" ref="AR1"/>
-  </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>